<commit_message>
update sprint 2 ggl sheets files
</commit_message>
<xml_diff>
--- a/Sprint 2/Detailed Log.xlsx
+++ b/Sprint 2/Detailed Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="182">
   <si>
     <t>Pritthiraj</t>
   </si>
@@ -306,6 +306,58 @@
 - assessslice to keep track of assessment info</t>
   </si>
   <si>
+    <t>#134</t>
+  </si>
+  <si>
+    <t>Design UI for Additional Dimensions</t>
+  </si>
+  <si>
+    <t>Update the peer assessment interface to include rating options for Conceptual Contribution, Practical Contribution, and Work Ethic, along with optional comment boxes for each.</t>
+  </si>
+  <si>
+    <t>#135</t>
+  </si>
+  <si>
+    <t>Implement Inputs Fields for Ratings</t>
+  </si>
+  <si>
+    <t>Add interactive input fields (5-point scales) for each dimension, ensuring proper layout and styling.</t>
+  </si>
+  <si>
+    <t>#136</t>
+  </si>
+  <si>
+    <t>Add Optional Comment Boxes</t>
+  </si>
+  <si>
+    <t>Provide text areas under each rating scale for students to input optional comments. Ensure the UI clearly indicates that these fields are optional.</t>
+  </si>
+  <si>
+    <t>#123</t>
+  </si>
+  <si>
+    <t>Sync Students Displayed with Backend via API calls + Team creation / deletion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    make the 'all students' and add csv buttons available to Teachers only
+    sync the students displayed wiht mySQL data
+    add api calls to csv upload button
+    team creation / deletion with database</t>
+  </si>
+  <si>
+    <t>#81</t>
+  </si>
+  <si>
+    <t>Add Confirmation Page</t>
+  </si>
+  <si>
+    <t>- Reference Number (like a transaction id)
+- Display new assessment (what it would look like)
+- Submit button
+- Cancel button
+- Print page button</t>
+  </si>
+  <si>
     <t>Viresh</t>
   </si>
   <si>
@@ -468,7 +520,7 @@
 done button</t>
   </si>
   <si>
-    <t>TASK 2.16 CI for frontend</t>
+    <t>TASK 2.14 CI for frontend</t>
   </si>
   <si>
     <t>must check that the app.tsx component loads</t>
@@ -681,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -727,7 +779,6 @@
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -1763,10 +1814,163 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18">
-      <c r="D18" s="15">
-        <f>SUM(D10:D17)</f>
-        <v>13</v>
-      </c>
+      <c r="A18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="F18" s="12">
+        <v>45591.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="E19" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="F19" s="12">
+        <v>45591.0</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="E20" s="11">
+        <v>10.0</v>
+      </c>
+      <c r="F20" s="12">
+        <v>45591.0</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>220.0</v>
+      </c>
+      <c r="F21" s="12">
+        <v>45591.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="E22" s="11">
+        <v>50.0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>45591.0</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1790,8 +1994,8 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="16" t="s">
-        <v>78</v>
+      <c r="A1" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1825,7 +2029,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>39</v>
@@ -1836,10 +2040,10 @@
         <v>4.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D4" s="6">
         <v>1.0</v>
@@ -1847,7 +2051,7 @@
       <c r="E4" s="6">
         <v>30.0</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>45555.0</v>
       </c>
       <c r="H4" s="5"/>
@@ -1857,10 +2061,10 @@
         <v>10.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D5" s="6">
         <v>1.0</v>
@@ -1868,7 +2072,7 @@
       <c r="E5" s="6">
         <v>15.0</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <v>45557.0</v>
       </c>
     </row>
@@ -1877,10 +2081,10 @@
         <v>11.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D6" s="6">
         <v>1.0</v>
@@ -1888,7 +2092,7 @@
       <c r="E6" s="6">
         <v>30.0</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="16">
         <v>45555.0</v>
       </c>
     </row>
@@ -1897,10 +2101,10 @@
         <v>14.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="D7" s="6">
         <v>2.0</v>
@@ -1908,7 +2112,7 @@
       <c r="E7" s="6">
         <v>90.0</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>45557.0</v>
       </c>
     </row>
@@ -1917,10 +2121,10 @@
         <v>16.0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="D8" s="6">
         <v>0.0</v>
@@ -1928,7 +2132,7 @@
       <c r="E8" s="6">
         <v>10.0</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>45558.0</v>
       </c>
     </row>
@@ -1937,10 +2141,10 @@
         <v>32.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="D9" s="6">
         <v>0.0</v>
@@ -1948,7 +2152,7 @@
       <c r="E9" s="6">
         <v>20.0</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="16">
         <v>45559.0</v>
       </c>
       <c r="H9" s="5"/>
@@ -1957,19 +2161,19 @@
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11">
       <c r="A11" s="6">
         <v>73.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D11" s="6">
         <v>2.0</v>
@@ -1977,7 +2181,7 @@
       <c r="E11" s="6">
         <v>45.0</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="16">
         <v>45572.0</v>
       </c>
     </row>
@@ -1986,10 +2190,10 @@
         <v>72.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="D12" s="6">
         <v>3.0</v>
@@ -1997,7 +2201,7 @@
       <c r="E12" s="6">
         <v>90.0</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <v>45572.0</v>
       </c>
     </row>
@@ -2006,10 +2210,10 @@
         <v>94.0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>97</v>
+        <v>111</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>112</v>
       </c>
       <c r="D13" s="6">
         <v>1.0</v>
@@ -2017,7 +2221,7 @@
       <c r="E13" s="6">
         <v>45.0</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="19">
         <v>45578.0</v>
       </c>
     </row>
@@ -2026,10 +2230,10 @@
         <v>97.0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="D14" s="6">
         <v>2.0</v>
@@ -2037,7 +2241,7 @@
       <c r="E14" s="6">
         <v>120.0</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="19">
         <v>45579.0</v>
       </c>
     </row>
@@ -2046,10 +2250,10 @@
         <v>98.0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="D15" s="6">
         <v>2.0</v>
@@ -2057,7 +2261,7 @@
       <c r="E15" s="6">
         <v>90.0</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="19">
         <v>45582.0</v>
       </c>
     </row>
@@ -2066,10 +2270,10 @@
         <v>100.0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="D16" s="6">
         <v>2.0</v>
@@ -2077,7 +2281,7 @@
       <c r="E16" s="6">
         <v>60.0</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="19">
         <v>45582.0</v>
       </c>
     </row>
@@ -2086,10 +2290,10 @@
         <v>113.0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="D17" s="6">
         <v>1.0</v>
@@ -2097,7 +2301,7 @@
       <c r="E17" s="6">
         <v>30.0</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="19">
         <v>45587.0</v>
       </c>
     </row>
@@ -2106,10 +2310,10 @@
         <v>114.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="D18" s="6">
         <v>1.0</v>
@@ -2117,38 +2321,38 @@
       <c r="E18" s="6">
         <v>30.0</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="19">
         <v>45587.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="18"/>
+      <c r="A20" s="17"/>
     </row>
     <row r="21">
-      <c r="A21" s="18"/>
+      <c r="A21" s="17"/>
     </row>
     <row r="22">
-      <c r="A22" s="18"/>
+      <c r="A22" s="17"/>
     </row>
     <row r="23">
-      <c r="A23" s="18"/>
+      <c r="A23" s="17"/>
     </row>
     <row r="24">
-      <c r="A24" s="18"/>
+      <c r="A24" s="17"/>
     </row>
     <row r="25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="17"/>
     </row>
     <row r="26">
-      <c r="A26" s="18"/>
+      <c r="A26" s="17"/>
     </row>
     <row r="27">
-      <c r="A27" s="18"/>
+      <c r="A27" s="17"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2172,7 +2376,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2217,10 +2421,10 @@
         <v>4.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="D4" s="2">
         <v>1.0</v>
@@ -2229,7 +2433,7 @@
         <v>50.0</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="H4" s="5"/>
     </row>
@@ -2238,10 +2442,10 @@
         <v>13.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="D5" s="2">
         <v>1.0</v>
@@ -2250,7 +2454,7 @@
         <v>15.0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6">
@@ -2258,16 +2462,16 @@
         <v>19.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="E6" s="2">
         <v>15.0</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7">
@@ -2275,10 +2479,10 @@
         <v>46.0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="D7" s="2">
         <v>2.0</v>
@@ -2287,7 +2491,7 @@
         <v>120.0</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8">
@@ -2300,10 +2504,10 @@
         <v>45.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="D9" s="2">
         <v>2.0</v>
@@ -2321,13 +2525,13 @@
         <v>61.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="D10" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E10" s="2">
         <v>50.0</v>
@@ -2341,10 +2545,10 @@
         <v>64.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="D11" s="2">
         <v>2.0</v>
@@ -2360,40 +2564,40 @@
       <c r="A12" s="2">
         <v>68.0</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>127</v>
+      <c r="B12" s="20" t="s">
+        <v>142</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="D12" s="2">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="E12" s="2">
-        <v>90.0</v>
+        <v>120.0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
         <v>96.0</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>130</v>
+      <c r="B13" s="20" t="s">
+        <v>145</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="D13" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E13" s="2">
-        <v>60.0</v>
+        <v>90.0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2417,7 +2621,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2435,87 +2639,87 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>133</v>
+      <c r="E3" s="21" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="22">
+      <c r="A4" s="21">
         <v>5.0</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="22">
+      <c r="B4" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="21">
         <v>60.0</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>135</v>
+      <c r="E4" s="21" t="s">
+        <v>150</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>8.0</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="22">
+      <c r="B5" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="21">
         <v>1.0</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>60.0</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>112</v>
+      <c r="E5" s="21" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="22">
+      <c r="A6" s="21">
         <v>19.0</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="22">
+      <c r="B6" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="21">
         <v>0.0</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <v>15.0</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>112</v>
+      <c r="E6" s="21" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>13.0</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="C7" s="22">
+      <c r="B7" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="21">
         <v>1.0</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>75.0</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>138</v>
+      <c r="E7" s="21" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="8">
@@ -2530,13 +2734,13 @@
         <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -2545,21 +2749,21 @@
         <v>62.0</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="D10" s="25">
+        <v>155</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="24">
         <v>3.0</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F10" s="26">
+        <v>157</v>
+      </c>
+      <c r="F10" s="25">
         <v>45575.0</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11">
@@ -2575,23 +2779,23 @@
       <c r="C14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="28">
+      <c r="A15" s="27">
         <v>60.0</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D15" s="28">
+        <v>159</v>
+      </c>
+      <c r="D15" s="27">
         <v>2.0</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="G15" s="8"/>
     </row>
@@ -2624,7 +2828,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2665,123 +2869,123 @@
       </c>
     </row>
     <row r="4" ht="44.25" customHeight="1">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>13.0</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="29">
+      <c r="C4" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="28">
         <v>0.0</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="30">
         <v>45555.0</v>
       </c>
       <c r="G4" s="12"/>
     </row>
     <row r="5" ht="32.25" customHeight="1">
-      <c r="A5" s="32">
+      <c r="A5" s="31">
         <v>12.0</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="32">
+      <c r="B5" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="31">
         <v>0.0</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="33">
         <v>45556.0</v>
       </c>
     </row>
     <row r="6" ht="31.5" customHeight="1">
-      <c r="A6" s="29">
+      <c r="A6" s="28">
         <v>6.0</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="30">
+      <c r="B6" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="29">
         <v>1.0</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="F6" s="35">
+      <c r="E6" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" s="34">
         <v>45561.0</v>
       </c>
     </row>
     <row r="7" ht="31.5" customHeight="1">
-      <c r="A7" s="29">
+      <c r="A7" s="28">
         <v>6.0</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="30">
+      <c r="B7" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="29">
         <v>1.0</v>
       </c>
-      <c r="E7" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="F7" s="35">
+      <c r="E7" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="34">
         <v>45562.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="29">
+      <c r="A8" s="28">
         <v>6.0</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="30">
+      <c r="B8" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" s="29">
         <v>2.0</v>
       </c>
-      <c r="E8" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="F8" s="35">
+      <c r="E8" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" s="34">
         <v>45563.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="29">
+      <c r="A9" s="28">
         <v>6.0</v>
       </c>
-      <c r="B9" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="D9" s="30">
+      <c r="B9" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="29">
         <v>0.0</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="34">
         <v>45564.0</v>
       </c>
       <c r="H9" s="5"/>
@@ -2796,18 +3000,18 @@
         <v>69.0</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="D11" s="10">
         <v>2.0</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="F11" s="36">
+        <v>176</v>
+      </c>
+      <c r="F11" s="35">
         <v>45582.0</v>
       </c>
       <c r="G11" s="8"/>
@@ -2820,18 +3024,18 @@
         <v>70.0</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="D12" s="10">
         <v>3.0</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="F12" s="36">
+        <v>179</v>
+      </c>
+      <c r="F12" s="35">
         <v>45585.0</v>
       </c>
       <c r="G12" s="8"/>
@@ -2844,16 +3048,16 @@
         <v>78.0</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="D13" s="10">
         <v>2.0</v>
       </c>
       <c r="E13" s="8"/>
-      <c r="F13" s="36">
+      <c r="F13" s="35">
         <v>45589.0</v>
       </c>
       <c r="G13" s="8"/>

</xml_diff>